<commit_message>
user can enter file path
</commit_message>
<xml_diff>
--- a/Final Test/Test_complete copy.xlsx
+++ b/Final Test/Test_complete copy.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amark/Documents/GitHub/SheetFormatter/Final Test/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2B0C01-5065-A546-958F-BB78680F7977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="23300" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="823">
   <si>
     <t>First Name</t>
   </si>
@@ -2494,8 +2488,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2517,21 +2511,6 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2573,15 +2552,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2589,14 +2565,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -2643,7 +2611,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2675,27 +2643,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2727,24 +2677,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2920,16 +2852,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V108"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:V101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2997,7 +2927,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3062,7 +2992,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -3121,7 +3051,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -3189,7 +3119,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -3257,7 +3187,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -3319,7 +3249,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -3387,7 +3317,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -3455,7 +3385,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -3523,7 +3453,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -3591,7 +3521,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -3659,7 +3589,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -3727,7 +3657,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -3795,7 +3725,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -3863,7 +3793,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -3931,7 +3861,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -3999,7 +3929,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -4067,7 +3997,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -4135,7 +4065,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -4203,7 +4133,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -4253,7 +4183,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -4318,7 +4248,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -4386,7 +4316,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -4451,7 +4381,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -4516,7 +4446,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -4581,7 +4511,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -4646,7 +4576,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -4711,7 +4641,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -4770,7 +4700,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -4835,7 +4765,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -4900,7 +4830,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -4959,7 +4889,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -5024,7 +4954,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -5092,7 +5022,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -5160,7 +5090,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -5222,7 +5152,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -5290,7 +5220,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -5358,7 +5288,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -5423,7 +5353,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22">
       <c r="A39" t="s">
         <v>59</v>
       </c>
@@ -5485,7 +5415,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22">
       <c r="A40" t="s">
         <v>60</v>
       </c>
@@ -5553,7 +5483,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22">
       <c r="A41" t="s">
         <v>61</v>
       </c>
@@ -5621,7 +5551,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -5689,7 +5619,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -5757,7 +5687,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -5813,7 +5743,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22">
       <c r="A45" t="s">
         <v>65</v>
       </c>
@@ -5878,7 +5808,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -5946,7 +5876,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22">
       <c r="A47" t="s">
         <v>67</v>
       </c>
@@ -6005,7 +5935,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22">
       <c r="A48" t="s">
         <v>68</v>
       </c>
@@ -6073,7 +6003,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:22">
       <c r="A49" t="s">
         <v>69</v>
       </c>
@@ -6141,7 +6071,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:22">
       <c r="A50" t="s">
         <v>70</v>
       </c>
@@ -6206,7 +6136,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:22">
       <c r="A51" t="s">
         <v>71</v>
       </c>
@@ -6274,7 +6204,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:22">
       <c r="A52" t="s">
         <v>72</v>
       </c>
@@ -6342,7 +6272,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:22">
       <c r="A53" t="s">
         <v>73</v>
       </c>
@@ -6407,7 +6337,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:22">
       <c r="A54" t="s">
         <v>74</v>
       </c>
@@ -6475,7 +6405,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:22">
       <c r="A55" t="s">
         <v>75</v>
       </c>
@@ -6543,7 +6473,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:22">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -6611,7 +6541,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:22">
       <c r="A57" t="s">
         <v>76</v>
       </c>
@@ -6679,7 +6609,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:22">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -6747,7 +6677,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:22">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -6815,7 +6745,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:22">
       <c r="A60" t="s">
         <v>79</v>
       </c>
@@ -6883,7 +6813,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:22">
       <c r="A61" t="s">
         <v>80</v>
       </c>
@@ -6951,7 +6881,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:22">
       <c r="A62" t="s">
         <v>81</v>
       </c>
@@ -7013,7 +6943,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:22">
       <c r="A63" t="s">
         <v>82</v>
       </c>
@@ -7072,7 +7002,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:22">
       <c r="A64" t="s">
         <v>83</v>
       </c>
@@ -7140,7 +7070,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:22">
       <c r="A65" t="s">
         <v>84</v>
       </c>
@@ -7208,7 +7138,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:22">
       <c r="A66" t="s">
         <v>85</v>
       </c>
@@ -7276,7 +7206,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:22">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -7344,7 +7274,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:22">
       <c r="A68" t="s">
         <v>87</v>
       </c>
@@ -7409,7 +7339,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:22">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -7477,7 +7407,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:22">
       <c r="A70" t="s">
         <v>88</v>
       </c>
@@ -7545,7 +7475,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:22">
       <c r="A71" t="s">
         <v>89</v>
       </c>
@@ -7613,7 +7543,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:22">
       <c r="A72" t="s">
         <v>90</v>
       </c>
@@ -7681,7 +7611,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:22">
       <c r="A73" t="s">
         <v>91</v>
       </c>
@@ -7749,7 +7679,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:22">
       <c r="A74" t="s">
         <v>92</v>
       </c>
@@ -7817,7 +7747,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:22">
       <c r="A75" t="s">
         <v>93</v>
       </c>
@@ -7882,7 +7812,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:22">
       <c r="A76" t="s">
         <v>94</v>
       </c>
@@ -7941,7 +7871,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:22">
       <c r="A77" t="s">
         <v>95</v>
       </c>
@@ -8003,7 +7933,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:22">
       <c r="A78" t="s">
         <v>96</v>
       </c>
@@ -8071,7 +8001,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:22">
       <c r="A79" t="s">
         <v>97</v>
       </c>
@@ -8139,7 +8069,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:22">
       <c r="A80" t="s">
         <v>98</v>
       </c>
@@ -8192,7 +8122,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:22">
       <c r="A81" t="s">
         <v>99</v>
       </c>
@@ -8260,7 +8190,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:22">
       <c r="A82" t="s">
         <v>100</v>
       </c>
@@ -8322,7 +8252,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:22">
       <c r="A83" t="s">
         <v>101</v>
       </c>
@@ -8378,7 +8308,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:22">
       <c r="A84" t="s">
         <v>88</v>
       </c>
@@ -8446,7 +8376,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:22">
       <c r="A85" t="s">
         <v>102</v>
       </c>
@@ -8514,7 +8444,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:22">
       <c r="A86" t="s">
         <v>53</v>
       </c>
@@ -8582,7 +8512,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:22">
       <c r="A87" t="s">
         <v>103</v>
       </c>
@@ -8650,7 +8580,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:22">
       <c r="A88" t="s">
         <v>104</v>
       </c>
@@ -8718,7 +8648,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:22">
       <c r="A89" t="s">
         <v>105</v>
       </c>
@@ -8783,7 +8713,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:22">
       <c r="A90" t="s">
         <v>106</v>
       </c>
@@ -8851,7 +8781,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:22">
       <c r="A91" t="s">
         <v>107</v>
       </c>
@@ -8919,7 +8849,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:22">
       <c r="A92" t="s">
         <v>108</v>
       </c>
@@ -8987,7 +8917,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:22">
       <c r="A93" t="s">
         <v>35</v>
       </c>
@@ -9055,7 +8985,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:22">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -9117,7 +9047,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:22">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -9185,7 +9115,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:22">
       <c r="A96" t="s">
         <v>111</v>
       </c>
@@ -9253,7 +9183,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:22">
       <c r="A97" t="s">
         <v>112</v>
       </c>
@@ -9318,7 +9248,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:22">
       <c r="A98" t="s">
         <v>113</v>
       </c>
@@ -9374,7 +9304,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:22">
       <c r="A99" t="s">
         <v>114</v>
       </c>
@@ -9436,7 +9366,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:22">
       <c r="A100" t="s">
         <v>115</v>
       </c>
@@ -9453,7 +9383,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:22">
       <c r="B101" t="s">
         <v>210</v>
       </c>
@@ -9467,899 +9397,482 @@
         <v>259</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A102" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="F102" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="G102" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="H102" s="3">
-        <v>390</v>
-      </c>
-      <c r="I102" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="J102" s="3" t="s">
-        <v>471</v>
-      </c>
-      <c r="K102" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="L102" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="M102" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="N102" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="O102" s="2" t="s">
-        <v>672</v>
-      </c>
-      <c r="P102" s="3" t="s">
-        <v>709</v>
-      </c>
-      <c r="Q102" s="3" t="s">
-        <v>747</v>
-      </c>
-      <c r="R102" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="S102" s="3" t="s">
-        <v>781</v>
-      </c>
-      <c r="T102" s="3" t="s">
-        <v>709</v>
-      </c>
-      <c r="U102" s="3" t="s">
-        <v>747</v>
-      </c>
-      <c r="V102" s="3" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="F103" s="3" t="s">
-        <v>426</v>
-      </c>
-      <c r="G103" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="H103" s="3">
-        <v>390</v>
-      </c>
-      <c r="I103" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="J103" s="3" t="s">
-        <v>471</v>
-      </c>
-      <c r="K103" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="L103" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="M103" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="N103" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="O103" s="2" t="s">
-        <v>672</v>
-      </c>
-      <c r="P103" s="3" t="s">
-        <v>709</v>
-      </c>
-      <c r="Q103" s="3" t="s">
-        <v>747</v>
-      </c>
-      <c r="R103" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="S103" s="3" t="s">
-        <v>781</v>
-      </c>
-      <c r="T103" s="3" t="s">
-        <v>709</v>
-      </c>
-      <c r="U103" s="3" t="s">
-        <v>747</v>
-      </c>
-      <c r="V103" s="3" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A104" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B104" s="3"/>
-      <c r="C104" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="G104" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="H104" s="3">
-        <v>130</v>
-      </c>
-      <c r="I104" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="J104" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="L104" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="M104" s="2" t="s">
-        <v>641</v>
-      </c>
-      <c r="N104" s="2" t="s">
-        <v>665</v>
-      </c>
-      <c r="O104" s="2" t="s">
-        <v>688</v>
-      </c>
-      <c r="P104" s="3" t="s">
-        <v>735</v>
-      </c>
-      <c r="Q104" s="3" t="s">
-        <v>760</v>
-      </c>
-      <c r="R104" s="3" t="s">
-        <v>766</v>
-      </c>
-      <c r="S104" s="3" t="s">
-        <v>799</v>
-      </c>
-      <c r="T104" s="3" t="s">
-        <v>814</v>
-      </c>
-      <c r="U104" s="3" t="s">
-        <v>821</v>
-      </c>
-      <c r="V104" s="3" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A105" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B105" s="3"/>
-      <c r="C105" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="F105" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="G105" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="H105" s="3">
-        <v>130</v>
-      </c>
-      <c r="I105" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="J105" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="K105" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="L105" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="M105" s="2" t="s">
-        <v>641</v>
-      </c>
-      <c r="N105" s="2" t="s">
-        <v>665</v>
-      </c>
-      <c r="O105" s="2" t="s">
-        <v>688</v>
-      </c>
-      <c r="P105" s="4"/>
-      <c r="Q105" s="4"/>
-      <c r="R105" s="3"/>
-      <c r="S105" s="3" t="s">
-        <v>799</v>
-      </c>
-      <c r="T105" s="3" t="s">
-        <v>814</v>
-      </c>
-      <c r="U105" s="3" t="s">
-        <v>821</v>
-      </c>
-      <c r="V105" s="3" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A106" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B106" s="3"/>
-      <c r="C106" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="F106" s="3"/>
-      <c r="G106" s="5">
-        <v>13200000000</v>
-      </c>
-      <c r="H106" s="3">
-        <v>130</v>
-      </c>
-      <c r="I106" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="J106" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="K106" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="L106" s="2" t="s">
-        <v>593</v>
-      </c>
-      <c r="M106" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="N106" s="2" t="s">
-        <v>648</v>
-      </c>
-      <c r="O106" s="2" t="s">
-        <v>670</v>
-      </c>
-      <c r="P106" s="3" t="s">
-        <v>736</v>
-      </c>
-      <c r="Q106" s="3" t="s">
-        <v>761</v>
-      </c>
-      <c r="R106" s="3" t="s">
-        <v>771</v>
-      </c>
-      <c r="S106" s="3" t="s">
-        <v>779</v>
-      </c>
-      <c r="T106" s="3" t="s">
-        <v>802</v>
-      </c>
-      <c r="U106" s="3" t="s">
-        <v>737</v>
-      </c>
-      <c r="V106" s="3" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A107" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="F107" s="3"/>
-      <c r="G107" s="3"/>
-      <c r="H107" s="3"/>
-      <c r="I107" s="3"/>
-      <c r="J107" s="3"/>
-      <c r="K107" s="3"/>
-      <c r="L107" s="3"/>
-      <c r="M107" s="3"/>
-      <c r="N107" s="3"/>
-      <c r="O107" s="3"/>
-      <c r="P107" s="3"/>
-      <c r="Q107" s="3"/>
-      <c r="R107" s="3"/>
-      <c r="S107" s="3"/>
-      <c r="T107" s="3"/>
-      <c r="U107" s="3"/>
-      <c r="V107" s="3"/>
-    </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A108" s="3"/>
-      <c r="B108" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="F108" s="3"/>
-      <c r="G108" s="3"/>
-      <c r="H108" s="3"/>
-      <c r="I108" s="3"/>
-      <c r="J108" s="3"/>
-      <c r="K108" s="3"/>
-      <c r="L108" s="3"/>
-      <c r="M108" s="3"/>
-      <c r="N108" s="3"/>
-      <c r="O108" s="3"/>
-      <c r="P108" s="3"/>
-      <c r="Q108" s="3"/>
-      <c r="R108" s="3"/>
-      <c r="S108" s="3"/>
-      <c r="T108" s="3"/>
-      <c r="U108" s="3"/>
-      <c r="V108" s="3"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="L2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="M2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="N2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="O2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="K3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="L3" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="M3" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="N3" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="O3" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="K4" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="L4" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="M4" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="N4" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="O4" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="K5" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="L5" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="M5" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="N5" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="O5" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="K6" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="L6" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="M6" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="N6" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="O6" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="K7" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="L7" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="M7" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="N7" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="O7" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="K8" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="L8" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="M8" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="N8" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="O8" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="K9" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="L9" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="M9" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="N9" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="O9" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="K10" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="L10" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="M10" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="N10" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="O10" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="K11" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="L11" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="M11" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="N11" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="O11" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="K12" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="L12" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="M12" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="N12" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="O12" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="K13" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="L13" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="M13" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="N13" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="O13" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="K14" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="L14" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="M14" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="N14" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="O14" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="K15" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="L15" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="M15" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="N15" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="O15" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="K16" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="L16" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="M16" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="N16" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="O16" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="K17" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="L17" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="M17" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="N17" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="O17" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="K18" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="L18" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="M18" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="N18" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="O18" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="K19" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="L19" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="M19" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="N19" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="O19" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="K20" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="L20" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="M20" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="K21" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="L21" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="M21" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="N21" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="K22" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="L22" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="M22" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="N22" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="O22" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="K23" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="L23" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="M23" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="N23" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="K24" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="L24" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="M24" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="N24" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="K25" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="L25" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="M25" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="N25" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="K26" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="L26" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="M26" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="N26" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="K27" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="L27" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="M27" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="N27" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="K28" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="L28" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="M28" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="N28" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="K29" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="L29" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="M29" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="N29" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="K30" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="L30" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="M30" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="N30" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="K31" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="L31" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="M31" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
-    <hyperlink ref="N31" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="O31" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="K32" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="L32" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="M32" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="O32" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
-    <hyperlink ref="K33" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="L33" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
-    <hyperlink ref="M33" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="N33" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="O33" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="K34" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="L34" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="M34" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="N34" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="O34" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
-    <hyperlink ref="K35" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="L35" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
-    <hyperlink ref="M35" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
-    <hyperlink ref="N35" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
-    <hyperlink ref="O35" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
-    <hyperlink ref="K36" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
-    <hyperlink ref="L36" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
-    <hyperlink ref="M36" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
-    <hyperlink ref="N36" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="O36" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
-    <hyperlink ref="K37" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="L37" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
-    <hyperlink ref="M37" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="N37" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
-    <hyperlink ref="O37" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="K38" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
-    <hyperlink ref="L38" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="M38" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
-    <hyperlink ref="N38" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
-    <hyperlink ref="O38" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
-    <hyperlink ref="K39" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
-    <hyperlink ref="L39" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
-    <hyperlink ref="M39" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
-    <hyperlink ref="N39" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
-    <hyperlink ref="O39" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
-    <hyperlink ref="K40" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
-    <hyperlink ref="L40" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
-    <hyperlink ref="M40" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
-    <hyperlink ref="N40" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
-    <hyperlink ref="O40" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
-    <hyperlink ref="K41" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
-    <hyperlink ref="L41" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
-    <hyperlink ref="M41" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
-    <hyperlink ref="N41" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
-    <hyperlink ref="O41" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
-    <hyperlink ref="K42" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
-    <hyperlink ref="L42" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
-    <hyperlink ref="M42" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
-    <hyperlink ref="N42" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
-    <hyperlink ref="O42" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
-    <hyperlink ref="K43" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
-    <hyperlink ref="L43" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
-    <hyperlink ref="M43" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="N43" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
-    <hyperlink ref="O43" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="K44" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
-    <hyperlink ref="L44" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="M44" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
-    <hyperlink ref="K45" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="L45" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
-    <hyperlink ref="M45" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
-    <hyperlink ref="N45" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
-    <hyperlink ref="O45" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="K46" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
-    <hyperlink ref="L46" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="M46" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
-    <hyperlink ref="N46" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="O46" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
-    <hyperlink ref="K47" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="L47" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
-    <hyperlink ref="M47" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="N47" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
-    <hyperlink ref="O47" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="K48" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
-    <hyperlink ref="L48" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="M48" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
-    <hyperlink ref="N48" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="O48" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
-    <hyperlink ref="K49" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="L49" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
-    <hyperlink ref="M49" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="N49" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
-    <hyperlink ref="O49" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
-    <hyperlink ref="K50" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
-    <hyperlink ref="L50" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
-    <hyperlink ref="M50" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
-    <hyperlink ref="N50" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
-    <hyperlink ref="O50" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
-    <hyperlink ref="K51" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
-    <hyperlink ref="L51" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
-    <hyperlink ref="M51" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
-    <hyperlink ref="N51" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
-    <hyperlink ref="O51" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
-    <hyperlink ref="K52" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
-    <hyperlink ref="L52" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
-    <hyperlink ref="M52" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
-    <hyperlink ref="N52" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
-    <hyperlink ref="O52" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
-    <hyperlink ref="K53" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
-    <hyperlink ref="L53" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
-    <hyperlink ref="M53" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
-    <hyperlink ref="N53" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
-    <hyperlink ref="O53" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
-    <hyperlink ref="K54" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
-    <hyperlink ref="L54" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
-    <hyperlink ref="M54" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
-    <hyperlink ref="N54" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
-    <hyperlink ref="O54" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
-    <hyperlink ref="K55" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
-    <hyperlink ref="L55" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
-    <hyperlink ref="M55" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
-    <hyperlink ref="N55" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
-    <hyperlink ref="O55" r:id="rId256" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
-    <hyperlink ref="K56" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
-    <hyperlink ref="L56" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
-    <hyperlink ref="M56" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
-    <hyperlink ref="N56" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
-    <hyperlink ref="O56" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
-    <hyperlink ref="K57" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
-    <hyperlink ref="L57" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
-    <hyperlink ref="M57" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
-    <hyperlink ref="N57" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
-    <hyperlink ref="O57" r:id="rId266" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
-    <hyperlink ref="K58" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
-    <hyperlink ref="L58" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
-    <hyperlink ref="M58" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
-    <hyperlink ref="N58" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
-    <hyperlink ref="O58" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
-    <hyperlink ref="K59" r:id="rId272" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
-    <hyperlink ref="L59" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
-    <hyperlink ref="M59" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
-    <hyperlink ref="N59" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
-    <hyperlink ref="O59" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
-    <hyperlink ref="K60" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
-    <hyperlink ref="L60" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
-    <hyperlink ref="M60" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
-    <hyperlink ref="N60" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
-    <hyperlink ref="O60" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
-    <hyperlink ref="K61" r:id="rId282" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
-    <hyperlink ref="L61" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
-    <hyperlink ref="M61" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
-    <hyperlink ref="N61" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
-    <hyperlink ref="O61" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
-    <hyperlink ref="K62" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
-    <hyperlink ref="L62" r:id="rId288" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
-    <hyperlink ref="M62" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
-    <hyperlink ref="N62" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
-    <hyperlink ref="O62" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
-    <hyperlink ref="K63" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
-    <hyperlink ref="L63" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
-    <hyperlink ref="M63" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
-    <hyperlink ref="N63" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
-    <hyperlink ref="O63" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
-    <hyperlink ref="K64" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
-    <hyperlink ref="L64" r:id="rId298" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
-    <hyperlink ref="M64" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
-    <hyperlink ref="N64" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
-    <hyperlink ref="O64" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
-    <hyperlink ref="K65" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
-    <hyperlink ref="L65" r:id="rId303" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
-    <hyperlink ref="M65" r:id="rId304" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
-    <hyperlink ref="N65" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
-    <hyperlink ref="O65" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
-    <hyperlink ref="K66" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
-    <hyperlink ref="L66" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
-    <hyperlink ref="M66" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
-    <hyperlink ref="N66" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
-    <hyperlink ref="O66" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
-    <hyperlink ref="K67" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
-    <hyperlink ref="L67" r:id="rId313" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
-    <hyperlink ref="M67" r:id="rId314" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
-    <hyperlink ref="N67" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
-    <hyperlink ref="O67" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
-    <hyperlink ref="K68" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
-    <hyperlink ref="L68" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
-    <hyperlink ref="M68" r:id="rId319" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
-    <hyperlink ref="N68" r:id="rId320" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
-    <hyperlink ref="O68" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
-    <hyperlink ref="K69" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
-    <hyperlink ref="L69" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
-    <hyperlink ref="M69" r:id="rId324" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
-    <hyperlink ref="N69" r:id="rId325" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
-    <hyperlink ref="O69" r:id="rId326" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
-    <hyperlink ref="K70" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
-    <hyperlink ref="L70" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
-    <hyperlink ref="M70" r:id="rId329" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
-    <hyperlink ref="N70" r:id="rId330" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
-    <hyperlink ref="O70" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
-    <hyperlink ref="K71" r:id="rId332" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
-    <hyperlink ref="L71" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
-    <hyperlink ref="M71" r:id="rId334" xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
-    <hyperlink ref="N71" r:id="rId335" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
-    <hyperlink ref="O71" r:id="rId336" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
-    <hyperlink ref="K72" r:id="rId337" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
-    <hyperlink ref="L72" r:id="rId338" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
-    <hyperlink ref="M72" r:id="rId339" xr:uid="{00000000-0004-0000-0000-000052010000}"/>
-    <hyperlink ref="N72" r:id="rId340" xr:uid="{00000000-0004-0000-0000-000053010000}"/>
-    <hyperlink ref="O72" r:id="rId341" xr:uid="{00000000-0004-0000-0000-000054010000}"/>
-    <hyperlink ref="K73" r:id="rId342" xr:uid="{00000000-0004-0000-0000-000055010000}"/>
-    <hyperlink ref="L73" r:id="rId343" xr:uid="{00000000-0004-0000-0000-000056010000}"/>
-    <hyperlink ref="M73" r:id="rId344" xr:uid="{00000000-0004-0000-0000-000057010000}"/>
-    <hyperlink ref="N73" r:id="rId345" xr:uid="{00000000-0004-0000-0000-000058010000}"/>
-    <hyperlink ref="O73" r:id="rId346" xr:uid="{00000000-0004-0000-0000-000059010000}"/>
-    <hyperlink ref="K74" r:id="rId347" xr:uid="{00000000-0004-0000-0000-00005A010000}"/>
-    <hyperlink ref="L74" r:id="rId348" xr:uid="{00000000-0004-0000-0000-00005B010000}"/>
-    <hyperlink ref="M74" r:id="rId349" xr:uid="{00000000-0004-0000-0000-00005C010000}"/>
-    <hyperlink ref="N74" r:id="rId350" xr:uid="{00000000-0004-0000-0000-00005D010000}"/>
-    <hyperlink ref="O74" r:id="rId351" xr:uid="{00000000-0004-0000-0000-00005E010000}"/>
-    <hyperlink ref="K75" r:id="rId352" xr:uid="{00000000-0004-0000-0000-00005F010000}"/>
-    <hyperlink ref="L75" r:id="rId353" xr:uid="{00000000-0004-0000-0000-000060010000}"/>
-    <hyperlink ref="M75" r:id="rId354" xr:uid="{00000000-0004-0000-0000-000061010000}"/>
-    <hyperlink ref="N75" r:id="rId355" xr:uid="{00000000-0004-0000-0000-000062010000}"/>
-    <hyperlink ref="O75" r:id="rId356" xr:uid="{00000000-0004-0000-0000-000063010000}"/>
-    <hyperlink ref="K76" r:id="rId357" xr:uid="{00000000-0004-0000-0000-000064010000}"/>
-    <hyperlink ref="L76" r:id="rId358" xr:uid="{00000000-0004-0000-0000-000065010000}"/>
-    <hyperlink ref="M76" r:id="rId359" xr:uid="{00000000-0004-0000-0000-000066010000}"/>
-    <hyperlink ref="N76" r:id="rId360" xr:uid="{00000000-0004-0000-0000-000067010000}"/>
-    <hyperlink ref="O76" r:id="rId361" xr:uid="{00000000-0004-0000-0000-000068010000}"/>
-    <hyperlink ref="K77" r:id="rId362" xr:uid="{00000000-0004-0000-0000-000069010000}"/>
-    <hyperlink ref="L77" r:id="rId363" xr:uid="{00000000-0004-0000-0000-00006A010000}"/>
-    <hyperlink ref="M77" r:id="rId364" xr:uid="{00000000-0004-0000-0000-00006B010000}"/>
-    <hyperlink ref="N77" r:id="rId365" xr:uid="{00000000-0004-0000-0000-00006C010000}"/>
-    <hyperlink ref="O77" r:id="rId366" xr:uid="{00000000-0004-0000-0000-00006D010000}"/>
-    <hyperlink ref="K78" r:id="rId367" xr:uid="{00000000-0004-0000-0000-00006E010000}"/>
-    <hyperlink ref="L78" r:id="rId368" xr:uid="{00000000-0004-0000-0000-00006F010000}"/>
-    <hyperlink ref="M78" r:id="rId369" xr:uid="{00000000-0004-0000-0000-000070010000}"/>
-    <hyperlink ref="N78" r:id="rId370" xr:uid="{00000000-0004-0000-0000-000071010000}"/>
-    <hyperlink ref="O78" r:id="rId371" xr:uid="{00000000-0004-0000-0000-000072010000}"/>
-    <hyperlink ref="K79" r:id="rId372" xr:uid="{00000000-0004-0000-0000-000073010000}"/>
-    <hyperlink ref="L79" r:id="rId373" xr:uid="{00000000-0004-0000-0000-000074010000}"/>
-    <hyperlink ref="M79" r:id="rId374" xr:uid="{00000000-0004-0000-0000-000075010000}"/>
-    <hyperlink ref="N79" r:id="rId375" xr:uid="{00000000-0004-0000-0000-000076010000}"/>
-    <hyperlink ref="O79" r:id="rId376" xr:uid="{00000000-0004-0000-0000-000077010000}"/>
-    <hyperlink ref="K80" r:id="rId377" xr:uid="{00000000-0004-0000-0000-000078010000}"/>
-    <hyperlink ref="L80" r:id="rId378" xr:uid="{00000000-0004-0000-0000-000079010000}"/>
-    <hyperlink ref="M80" r:id="rId379" xr:uid="{00000000-0004-0000-0000-00007A010000}"/>
-    <hyperlink ref="K81" r:id="rId380" xr:uid="{00000000-0004-0000-0000-00007B010000}"/>
-    <hyperlink ref="L81" r:id="rId381" xr:uid="{00000000-0004-0000-0000-00007C010000}"/>
-    <hyperlink ref="M81" r:id="rId382" xr:uid="{00000000-0004-0000-0000-00007D010000}"/>
-    <hyperlink ref="N81" r:id="rId383" xr:uid="{00000000-0004-0000-0000-00007E010000}"/>
-    <hyperlink ref="O81" r:id="rId384" xr:uid="{00000000-0004-0000-0000-00007F010000}"/>
-    <hyperlink ref="K82" r:id="rId385" xr:uid="{00000000-0004-0000-0000-000080010000}"/>
-    <hyperlink ref="L82" r:id="rId386" xr:uid="{00000000-0004-0000-0000-000081010000}"/>
-    <hyperlink ref="M82" r:id="rId387" xr:uid="{00000000-0004-0000-0000-000082010000}"/>
-    <hyperlink ref="N82" r:id="rId388" xr:uid="{00000000-0004-0000-0000-000083010000}"/>
-    <hyperlink ref="O82" r:id="rId389" xr:uid="{00000000-0004-0000-0000-000084010000}"/>
-    <hyperlink ref="K83" r:id="rId390" xr:uid="{00000000-0004-0000-0000-000085010000}"/>
-    <hyperlink ref="L83" r:id="rId391" xr:uid="{00000000-0004-0000-0000-000086010000}"/>
-    <hyperlink ref="M83" r:id="rId392" xr:uid="{00000000-0004-0000-0000-000087010000}"/>
-    <hyperlink ref="N83" r:id="rId393" xr:uid="{00000000-0004-0000-0000-000088010000}"/>
-    <hyperlink ref="O83" r:id="rId394" xr:uid="{00000000-0004-0000-0000-000089010000}"/>
-    <hyperlink ref="K84" r:id="rId395" xr:uid="{00000000-0004-0000-0000-00008A010000}"/>
-    <hyperlink ref="L84" r:id="rId396" xr:uid="{00000000-0004-0000-0000-00008B010000}"/>
-    <hyperlink ref="M84" r:id="rId397" xr:uid="{00000000-0004-0000-0000-00008C010000}"/>
-    <hyperlink ref="N84" r:id="rId398" xr:uid="{00000000-0004-0000-0000-00008D010000}"/>
-    <hyperlink ref="O84" r:id="rId399" xr:uid="{00000000-0004-0000-0000-00008E010000}"/>
-    <hyperlink ref="K85" r:id="rId400" xr:uid="{00000000-0004-0000-0000-00008F010000}"/>
-    <hyperlink ref="L85" r:id="rId401" xr:uid="{00000000-0004-0000-0000-000090010000}"/>
-    <hyperlink ref="M85" r:id="rId402" xr:uid="{00000000-0004-0000-0000-000091010000}"/>
-    <hyperlink ref="N85" r:id="rId403" xr:uid="{00000000-0004-0000-0000-000092010000}"/>
-    <hyperlink ref="O85" r:id="rId404" xr:uid="{00000000-0004-0000-0000-000093010000}"/>
-    <hyperlink ref="K86" r:id="rId405" xr:uid="{00000000-0004-0000-0000-000094010000}"/>
-    <hyperlink ref="L86" r:id="rId406" xr:uid="{00000000-0004-0000-0000-000095010000}"/>
-    <hyperlink ref="M86" r:id="rId407" xr:uid="{00000000-0004-0000-0000-000096010000}"/>
-    <hyperlink ref="N86" r:id="rId408" xr:uid="{00000000-0004-0000-0000-000097010000}"/>
-    <hyperlink ref="O86" r:id="rId409" xr:uid="{00000000-0004-0000-0000-000098010000}"/>
-    <hyperlink ref="K87" r:id="rId410" xr:uid="{00000000-0004-0000-0000-000099010000}"/>
-    <hyperlink ref="L87" r:id="rId411" xr:uid="{00000000-0004-0000-0000-00009A010000}"/>
-    <hyperlink ref="M87" r:id="rId412" xr:uid="{00000000-0004-0000-0000-00009B010000}"/>
-    <hyperlink ref="N87" r:id="rId413" xr:uid="{00000000-0004-0000-0000-00009C010000}"/>
-    <hyperlink ref="O87" r:id="rId414" xr:uid="{00000000-0004-0000-0000-00009D010000}"/>
-    <hyperlink ref="K88" r:id="rId415" xr:uid="{00000000-0004-0000-0000-00009E010000}"/>
-    <hyperlink ref="L88" r:id="rId416" xr:uid="{00000000-0004-0000-0000-00009F010000}"/>
-    <hyperlink ref="M88" r:id="rId417" xr:uid="{00000000-0004-0000-0000-0000A0010000}"/>
-    <hyperlink ref="N88" r:id="rId418" xr:uid="{00000000-0004-0000-0000-0000A1010000}"/>
-    <hyperlink ref="O88" r:id="rId419" xr:uid="{00000000-0004-0000-0000-0000A2010000}"/>
-    <hyperlink ref="K89" r:id="rId420" xr:uid="{00000000-0004-0000-0000-0000A3010000}"/>
-    <hyperlink ref="L89" r:id="rId421" xr:uid="{00000000-0004-0000-0000-0000A4010000}"/>
-    <hyperlink ref="M89" r:id="rId422" xr:uid="{00000000-0004-0000-0000-0000A5010000}"/>
-    <hyperlink ref="N89" r:id="rId423" xr:uid="{00000000-0004-0000-0000-0000A6010000}"/>
-    <hyperlink ref="O89" r:id="rId424" xr:uid="{00000000-0004-0000-0000-0000A7010000}"/>
-    <hyperlink ref="K90" r:id="rId425" xr:uid="{00000000-0004-0000-0000-0000A8010000}"/>
-    <hyperlink ref="L90" r:id="rId426" xr:uid="{00000000-0004-0000-0000-0000A9010000}"/>
-    <hyperlink ref="M90" r:id="rId427" xr:uid="{00000000-0004-0000-0000-0000AA010000}"/>
-    <hyperlink ref="N90" r:id="rId428" xr:uid="{00000000-0004-0000-0000-0000AB010000}"/>
-    <hyperlink ref="O90" r:id="rId429" xr:uid="{00000000-0004-0000-0000-0000AC010000}"/>
-    <hyperlink ref="K91" r:id="rId430" xr:uid="{00000000-0004-0000-0000-0000AD010000}"/>
-    <hyperlink ref="L91" r:id="rId431" xr:uid="{00000000-0004-0000-0000-0000AE010000}"/>
-    <hyperlink ref="M91" r:id="rId432" xr:uid="{00000000-0004-0000-0000-0000AF010000}"/>
-    <hyperlink ref="N91" r:id="rId433" xr:uid="{00000000-0004-0000-0000-0000B0010000}"/>
-    <hyperlink ref="O91" r:id="rId434" xr:uid="{00000000-0004-0000-0000-0000B1010000}"/>
-    <hyperlink ref="K92" r:id="rId435" xr:uid="{00000000-0004-0000-0000-0000B2010000}"/>
-    <hyperlink ref="L92" r:id="rId436" xr:uid="{00000000-0004-0000-0000-0000B3010000}"/>
-    <hyperlink ref="M92" r:id="rId437" xr:uid="{00000000-0004-0000-0000-0000B4010000}"/>
-    <hyperlink ref="N92" r:id="rId438" xr:uid="{00000000-0004-0000-0000-0000B5010000}"/>
-    <hyperlink ref="O92" r:id="rId439" xr:uid="{00000000-0004-0000-0000-0000B6010000}"/>
-    <hyperlink ref="K93" r:id="rId440" xr:uid="{00000000-0004-0000-0000-0000B7010000}"/>
-    <hyperlink ref="L93" r:id="rId441" xr:uid="{00000000-0004-0000-0000-0000B8010000}"/>
-    <hyperlink ref="M93" r:id="rId442" xr:uid="{00000000-0004-0000-0000-0000B9010000}"/>
-    <hyperlink ref="N93" r:id="rId443" xr:uid="{00000000-0004-0000-0000-0000BA010000}"/>
-    <hyperlink ref="O93" r:id="rId444" xr:uid="{00000000-0004-0000-0000-0000BB010000}"/>
-    <hyperlink ref="K94" r:id="rId445" xr:uid="{00000000-0004-0000-0000-0000BC010000}"/>
-    <hyperlink ref="L94" r:id="rId446" xr:uid="{00000000-0004-0000-0000-0000BD010000}"/>
-    <hyperlink ref="M94" r:id="rId447" xr:uid="{00000000-0004-0000-0000-0000BE010000}"/>
-    <hyperlink ref="N94" r:id="rId448" xr:uid="{00000000-0004-0000-0000-0000BF010000}"/>
-    <hyperlink ref="O94" r:id="rId449" xr:uid="{00000000-0004-0000-0000-0000C0010000}"/>
-    <hyperlink ref="K95" r:id="rId450" xr:uid="{00000000-0004-0000-0000-0000C1010000}"/>
-    <hyperlink ref="L95" r:id="rId451" xr:uid="{00000000-0004-0000-0000-0000C2010000}"/>
-    <hyperlink ref="M95" r:id="rId452" xr:uid="{00000000-0004-0000-0000-0000C3010000}"/>
-    <hyperlink ref="N95" r:id="rId453" xr:uid="{00000000-0004-0000-0000-0000C4010000}"/>
-    <hyperlink ref="O95" r:id="rId454" xr:uid="{00000000-0004-0000-0000-0000C5010000}"/>
-    <hyperlink ref="K96" r:id="rId455" xr:uid="{00000000-0004-0000-0000-0000C6010000}"/>
-    <hyperlink ref="L96" r:id="rId456" xr:uid="{00000000-0004-0000-0000-0000C7010000}"/>
-    <hyperlink ref="M96" r:id="rId457" xr:uid="{00000000-0004-0000-0000-0000C8010000}"/>
-    <hyperlink ref="N96" r:id="rId458" xr:uid="{00000000-0004-0000-0000-0000C9010000}"/>
-    <hyperlink ref="O96" r:id="rId459" xr:uid="{00000000-0004-0000-0000-0000CA010000}"/>
-    <hyperlink ref="K97" r:id="rId460" xr:uid="{00000000-0004-0000-0000-0000CB010000}"/>
-    <hyperlink ref="L97" r:id="rId461" xr:uid="{00000000-0004-0000-0000-0000CC010000}"/>
-    <hyperlink ref="M97" r:id="rId462" xr:uid="{00000000-0004-0000-0000-0000CD010000}"/>
-    <hyperlink ref="N97" r:id="rId463" xr:uid="{00000000-0004-0000-0000-0000CE010000}"/>
-    <hyperlink ref="O97" r:id="rId464" xr:uid="{00000000-0004-0000-0000-0000CF010000}"/>
-    <hyperlink ref="K98" r:id="rId465" xr:uid="{00000000-0004-0000-0000-0000D0010000}"/>
-    <hyperlink ref="L98" r:id="rId466" xr:uid="{00000000-0004-0000-0000-0000D1010000}"/>
-    <hyperlink ref="M98" r:id="rId467" xr:uid="{00000000-0004-0000-0000-0000D2010000}"/>
-    <hyperlink ref="N98" r:id="rId468" xr:uid="{00000000-0004-0000-0000-0000D3010000}"/>
-    <hyperlink ref="O98" r:id="rId469" xr:uid="{00000000-0004-0000-0000-0000D4010000}"/>
-    <hyperlink ref="K99" r:id="rId470" xr:uid="{00000000-0004-0000-0000-0000D5010000}"/>
-    <hyperlink ref="L99" r:id="rId471" xr:uid="{00000000-0004-0000-0000-0000D6010000}"/>
-    <hyperlink ref="M99" r:id="rId472" xr:uid="{00000000-0004-0000-0000-0000D7010000}"/>
-    <hyperlink ref="N99" r:id="rId473" xr:uid="{00000000-0004-0000-0000-0000D8010000}"/>
-    <hyperlink ref="O99" r:id="rId474" xr:uid="{00000000-0004-0000-0000-0000D9010000}"/>
-    <hyperlink ref="K102" r:id="rId475" xr:uid="{8E006870-1B31-B240-960A-AE3725E2230B}"/>
-    <hyperlink ref="L102" r:id="rId476" display="http://www.ebq.com/" xr:uid="{581F0857-E15A-F842-BC46-A706E207A0A1}"/>
-    <hyperlink ref="M102" r:id="rId477" xr:uid="{472A08CB-65A3-4347-A571-31860A80CDFA}"/>
-    <hyperlink ref="N102" r:id="rId478" xr:uid="{307A7EBF-05C2-D048-9E62-B76B1571B80D}"/>
-    <hyperlink ref="O102" r:id="rId479" xr:uid="{17AAC995-E57F-BE44-B9BB-39F62EE2939F}"/>
-    <hyperlink ref="K103" r:id="rId480" xr:uid="{F8A074A1-F3FF-DF4C-B6C1-482DA7408241}"/>
-    <hyperlink ref="L103" r:id="rId481" display="http://www.ebq.com/" xr:uid="{25A55021-5CAE-F64B-BD45-C30E5848ED2F}"/>
-    <hyperlink ref="M103" r:id="rId482" xr:uid="{A48D447A-19EF-AA4F-854D-290AAA312AA7}"/>
-    <hyperlink ref="N103" r:id="rId483" xr:uid="{3F9B770C-E6DF-ED4A-8F4D-5AFA5EA7C67B}"/>
-    <hyperlink ref="O103" r:id="rId484" xr:uid="{8DE0FD5C-9F5A-9748-B439-8CE46348FA3C}"/>
-    <hyperlink ref="K104" r:id="rId485" xr:uid="{E51988CE-D154-BC4B-A22E-911936928166}"/>
-    <hyperlink ref="L104" r:id="rId486" display="http://www.theglobalassociates.com/" xr:uid="{8A4E35C5-15FC-7343-B79A-1C60BF3BBFD4}"/>
-    <hyperlink ref="M104" r:id="rId487" xr:uid="{F9CC6539-36E7-3E4C-8C3F-0A0EFF5C2156}"/>
-    <hyperlink ref="N104" r:id="rId488" xr:uid="{9D246040-D99B-8A4A-9C8E-688EBB99055E}"/>
-    <hyperlink ref="O104" r:id="rId489" xr:uid="{65CB7040-1D2F-4C4E-AB81-4971C34E0658}"/>
-    <hyperlink ref="K105" r:id="rId490" xr:uid="{7AD226F3-3650-5C45-9029-2CCE0951F266}"/>
-    <hyperlink ref="L105" r:id="rId491" display="http://www.theglobalassociates.com/" xr:uid="{44AC4065-D2D5-5F47-B3BF-442D4C65AA57}"/>
-    <hyperlink ref="M105" r:id="rId492" xr:uid="{EF84D3AF-0CED-2140-B09C-07C3966B671D}"/>
-    <hyperlink ref="N105" r:id="rId493" xr:uid="{267902EC-B6FB-BD4C-BFF2-4270DC0663B5}"/>
-    <hyperlink ref="O105" r:id="rId494" xr:uid="{F57D6F64-D8E1-104D-84CE-59BB078CD12F}"/>
-    <hyperlink ref="K106" r:id="rId495" xr:uid="{035D93AB-9CB4-2644-B38A-5D2DDF8E1E78}"/>
-    <hyperlink ref="L106" r:id="rId496" display="http://www.taskdrive.com/" xr:uid="{B5A03513-0824-BF44-87B9-2CFF557A72E0}"/>
-    <hyperlink ref="M106" r:id="rId497" xr:uid="{FFBD7E41-A4A0-EA42-B5E8-2C7513472620}"/>
-    <hyperlink ref="N106" r:id="rId498" xr:uid="{1CADAE5D-ABEC-4B4E-8809-1A1F46EFC093}"/>
-    <hyperlink ref="O106" r:id="rId499" xr:uid="{8E55BCEE-B09E-7F4E-81DA-E2826DB4189D}"/>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="L2" r:id="rId2"/>
+    <hyperlink ref="M2" r:id="rId3"/>
+    <hyperlink ref="N2" r:id="rId4"/>
+    <hyperlink ref="O2" r:id="rId5"/>
+    <hyperlink ref="K3" r:id="rId6"/>
+    <hyperlink ref="L3" r:id="rId7"/>
+    <hyperlink ref="M3" r:id="rId8"/>
+    <hyperlink ref="N3" r:id="rId9"/>
+    <hyperlink ref="O3" r:id="rId10"/>
+    <hyperlink ref="K4" r:id="rId11"/>
+    <hyperlink ref="L4" r:id="rId12"/>
+    <hyperlink ref="M4" r:id="rId13"/>
+    <hyperlink ref="N4" r:id="rId14"/>
+    <hyperlink ref="O4" r:id="rId15"/>
+    <hyperlink ref="K5" r:id="rId16"/>
+    <hyperlink ref="L5" r:id="rId17"/>
+    <hyperlink ref="M5" r:id="rId18"/>
+    <hyperlink ref="N5" r:id="rId19"/>
+    <hyperlink ref="O5" r:id="rId20"/>
+    <hyperlink ref="K6" r:id="rId21"/>
+    <hyperlink ref="L6" r:id="rId22"/>
+    <hyperlink ref="M6" r:id="rId23"/>
+    <hyperlink ref="N6" r:id="rId24"/>
+    <hyperlink ref="O6" r:id="rId25"/>
+    <hyperlink ref="K7" r:id="rId26"/>
+    <hyperlink ref="L7" r:id="rId27"/>
+    <hyperlink ref="M7" r:id="rId28"/>
+    <hyperlink ref="N7" r:id="rId29"/>
+    <hyperlink ref="O7" r:id="rId30"/>
+    <hyperlink ref="K8" r:id="rId31"/>
+    <hyperlink ref="L8" r:id="rId32"/>
+    <hyperlink ref="M8" r:id="rId33"/>
+    <hyperlink ref="N8" r:id="rId34"/>
+    <hyperlink ref="O8" r:id="rId35"/>
+    <hyperlink ref="K9" r:id="rId36"/>
+    <hyperlink ref="L9" r:id="rId37"/>
+    <hyperlink ref="M9" r:id="rId38"/>
+    <hyperlink ref="N9" r:id="rId39"/>
+    <hyperlink ref="O9" r:id="rId40"/>
+    <hyperlink ref="K10" r:id="rId41"/>
+    <hyperlink ref="L10" r:id="rId42"/>
+    <hyperlink ref="M10" r:id="rId43"/>
+    <hyperlink ref="N10" r:id="rId44"/>
+    <hyperlink ref="O10" r:id="rId45"/>
+    <hyperlink ref="K11" r:id="rId46"/>
+    <hyperlink ref="L11" r:id="rId47"/>
+    <hyperlink ref="M11" r:id="rId48"/>
+    <hyperlink ref="N11" r:id="rId49"/>
+    <hyperlink ref="O11" r:id="rId50"/>
+    <hyperlink ref="K12" r:id="rId51"/>
+    <hyperlink ref="L12" r:id="rId52"/>
+    <hyperlink ref="M12" r:id="rId53"/>
+    <hyperlink ref="N12" r:id="rId54"/>
+    <hyperlink ref="O12" r:id="rId55"/>
+    <hyperlink ref="K13" r:id="rId56"/>
+    <hyperlink ref="L13" r:id="rId57"/>
+    <hyperlink ref="M13" r:id="rId58"/>
+    <hyperlink ref="N13" r:id="rId59"/>
+    <hyperlink ref="O13" r:id="rId60"/>
+    <hyperlink ref="K14" r:id="rId61"/>
+    <hyperlink ref="L14" r:id="rId62"/>
+    <hyperlink ref="M14" r:id="rId63"/>
+    <hyperlink ref="N14" r:id="rId64"/>
+    <hyperlink ref="O14" r:id="rId65"/>
+    <hyperlink ref="K15" r:id="rId66"/>
+    <hyperlink ref="L15" r:id="rId67"/>
+    <hyperlink ref="M15" r:id="rId68"/>
+    <hyperlink ref="N15" r:id="rId69"/>
+    <hyperlink ref="O15" r:id="rId70"/>
+    <hyperlink ref="K16" r:id="rId71"/>
+    <hyperlink ref="L16" r:id="rId72"/>
+    <hyperlink ref="M16" r:id="rId73"/>
+    <hyperlink ref="N16" r:id="rId74"/>
+    <hyperlink ref="O16" r:id="rId75"/>
+    <hyperlink ref="K17" r:id="rId76"/>
+    <hyperlink ref="L17" r:id="rId77"/>
+    <hyperlink ref="M17" r:id="rId78"/>
+    <hyperlink ref="N17" r:id="rId79"/>
+    <hyperlink ref="O17" r:id="rId80"/>
+    <hyperlink ref="K18" r:id="rId81"/>
+    <hyperlink ref="L18" r:id="rId82"/>
+    <hyperlink ref="M18" r:id="rId83"/>
+    <hyperlink ref="N18" r:id="rId84"/>
+    <hyperlink ref="O18" r:id="rId85"/>
+    <hyperlink ref="K19" r:id="rId86"/>
+    <hyperlink ref="L19" r:id="rId87"/>
+    <hyperlink ref="M19" r:id="rId88"/>
+    <hyperlink ref="N19" r:id="rId89"/>
+    <hyperlink ref="O19" r:id="rId90"/>
+    <hyperlink ref="K20" r:id="rId91"/>
+    <hyperlink ref="L20" r:id="rId92"/>
+    <hyperlink ref="M20" r:id="rId93"/>
+    <hyperlink ref="K21" r:id="rId94"/>
+    <hyperlink ref="L21" r:id="rId95"/>
+    <hyperlink ref="M21" r:id="rId96"/>
+    <hyperlink ref="N21" r:id="rId97"/>
+    <hyperlink ref="K22" r:id="rId98"/>
+    <hyperlink ref="L22" r:id="rId99"/>
+    <hyperlink ref="M22" r:id="rId100"/>
+    <hyperlink ref="N22" r:id="rId101"/>
+    <hyperlink ref="O22" r:id="rId102"/>
+    <hyperlink ref="K23" r:id="rId103"/>
+    <hyperlink ref="L23" r:id="rId104"/>
+    <hyperlink ref="M23" r:id="rId105"/>
+    <hyperlink ref="N23" r:id="rId106"/>
+    <hyperlink ref="K24" r:id="rId107"/>
+    <hyperlink ref="L24" r:id="rId108"/>
+    <hyperlink ref="M24" r:id="rId109"/>
+    <hyperlink ref="N24" r:id="rId110"/>
+    <hyperlink ref="K25" r:id="rId111"/>
+    <hyperlink ref="L25" r:id="rId112"/>
+    <hyperlink ref="M25" r:id="rId113"/>
+    <hyperlink ref="N25" r:id="rId114"/>
+    <hyperlink ref="K26" r:id="rId115"/>
+    <hyperlink ref="L26" r:id="rId116"/>
+    <hyperlink ref="M26" r:id="rId117"/>
+    <hyperlink ref="N26" r:id="rId118"/>
+    <hyperlink ref="K27" r:id="rId119"/>
+    <hyperlink ref="L27" r:id="rId120"/>
+    <hyperlink ref="M27" r:id="rId121"/>
+    <hyperlink ref="N27" r:id="rId122"/>
+    <hyperlink ref="K28" r:id="rId123"/>
+    <hyperlink ref="L28" r:id="rId124"/>
+    <hyperlink ref="M28" r:id="rId125"/>
+    <hyperlink ref="N28" r:id="rId126"/>
+    <hyperlink ref="K29" r:id="rId127"/>
+    <hyperlink ref="L29" r:id="rId128"/>
+    <hyperlink ref="M29" r:id="rId129"/>
+    <hyperlink ref="N29" r:id="rId130"/>
+    <hyperlink ref="K30" r:id="rId131"/>
+    <hyperlink ref="L30" r:id="rId132"/>
+    <hyperlink ref="M30" r:id="rId133"/>
+    <hyperlink ref="N30" r:id="rId134"/>
+    <hyperlink ref="K31" r:id="rId135"/>
+    <hyperlink ref="L31" r:id="rId136"/>
+    <hyperlink ref="M31" r:id="rId137"/>
+    <hyperlink ref="N31" r:id="rId138"/>
+    <hyperlink ref="O31" r:id="rId139"/>
+    <hyperlink ref="K32" r:id="rId140"/>
+    <hyperlink ref="L32" r:id="rId141"/>
+    <hyperlink ref="M32" r:id="rId142"/>
+    <hyperlink ref="O32" r:id="rId143"/>
+    <hyperlink ref="K33" r:id="rId144"/>
+    <hyperlink ref="L33" r:id="rId145"/>
+    <hyperlink ref="M33" r:id="rId146"/>
+    <hyperlink ref="N33" r:id="rId147"/>
+    <hyperlink ref="O33" r:id="rId148"/>
+    <hyperlink ref="K34" r:id="rId149"/>
+    <hyperlink ref="L34" r:id="rId150"/>
+    <hyperlink ref="M34" r:id="rId151"/>
+    <hyperlink ref="N34" r:id="rId152"/>
+    <hyperlink ref="O34" r:id="rId153"/>
+    <hyperlink ref="K35" r:id="rId154"/>
+    <hyperlink ref="L35" r:id="rId155"/>
+    <hyperlink ref="M35" r:id="rId156"/>
+    <hyperlink ref="N35" r:id="rId157"/>
+    <hyperlink ref="O35" r:id="rId158"/>
+    <hyperlink ref="K36" r:id="rId159"/>
+    <hyperlink ref="L36" r:id="rId160"/>
+    <hyperlink ref="M36" r:id="rId161"/>
+    <hyperlink ref="N36" r:id="rId162"/>
+    <hyperlink ref="O36" r:id="rId163"/>
+    <hyperlink ref="K37" r:id="rId164"/>
+    <hyperlink ref="L37" r:id="rId165"/>
+    <hyperlink ref="M37" r:id="rId166"/>
+    <hyperlink ref="N37" r:id="rId167"/>
+    <hyperlink ref="O37" r:id="rId168"/>
+    <hyperlink ref="K38" r:id="rId169"/>
+    <hyperlink ref="L38" r:id="rId170"/>
+    <hyperlink ref="M38" r:id="rId171"/>
+    <hyperlink ref="N38" r:id="rId172"/>
+    <hyperlink ref="O38" r:id="rId173"/>
+    <hyperlink ref="K39" r:id="rId174"/>
+    <hyperlink ref="L39" r:id="rId175"/>
+    <hyperlink ref="M39" r:id="rId176"/>
+    <hyperlink ref="N39" r:id="rId177"/>
+    <hyperlink ref="O39" r:id="rId178"/>
+    <hyperlink ref="K40" r:id="rId179"/>
+    <hyperlink ref="L40" r:id="rId180"/>
+    <hyperlink ref="M40" r:id="rId181"/>
+    <hyperlink ref="N40" r:id="rId182"/>
+    <hyperlink ref="O40" r:id="rId183"/>
+    <hyperlink ref="K41" r:id="rId184"/>
+    <hyperlink ref="L41" r:id="rId185"/>
+    <hyperlink ref="M41" r:id="rId186"/>
+    <hyperlink ref="N41" r:id="rId187"/>
+    <hyperlink ref="O41" r:id="rId188"/>
+    <hyperlink ref="K42" r:id="rId189"/>
+    <hyperlink ref="L42" r:id="rId190"/>
+    <hyperlink ref="M42" r:id="rId191"/>
+    <hyperlink ref="N42" r:id="rId192"/>
+    <hyperlink ref="O42" r:id="rId193"/>
+    <hyperlink ref="K43" r:id="rId194"/>
+    <hyperlink ref="L43" r:id="rId195"/>
+    <hyperlink ref="M43" r:id="rId196"/>
+    <hyperlink ref="N43" r:id="rId197"/>
+    <hyperlink ref="O43" r:id="rId198"/>
+    <hyperlink ref="K44" r:id="rId199"/>
+    <hyperlink ref="L44" r:id="rId200"/>
+    <hyperlink ref="M44" r:id="rId201"/>
+    <hyperlink ref="K45" r:id="rId202"/>
+    <hyperlink ref="L45" r:id="rId203"/>
+    <hyperlink ref="M45" r:id="rId204"/>
+    <hyperlink ref="N45" r:id="rId205"/>
+    <hyperlink ref="O45" r:id="rId206"/>
+    <hyperlink ref="K46" r:id="rId207"/>
+    <hyperlink ref="L46" r:id="rId208"/>
+    <hyperlink ref="M46" r:id="rId209"/>
+    <hyperlink ref="N46" r:id="rId210"/>
+    <hyperlink ref="O46" r:id="rId211"/>
+    <hyperlink ref="K47" r:id="rId212"/>
+    <hyperlink ref="L47" r:id="rId213"/>
+    <hyperlink ref="M47" r:id="rId214"/>
+    <hyperlink ref="N47" r:id="rId215"/>
+    <hyperlink ref="O47" r:id="rId216"/>
+    <hyperlink ref="K48" r:id="rId217"/>
+    <hyperlink ref="L48" r:id="rId218"/>
+    <hyperlink ref="M48" r:id="rId219"/>
+    <hyperlink ref="N48" r:id="rId220"/>
+    <hyperlink ref="O48" r:id="rId221"/>
+    <hyperlink ref="K49" r:id="rId222"/>
+    <hyperlink ref="L49" r:id="rId223"/>
+    <hyperlink ref="M49" r:id="rId224"/>
+    <hyperlink ref="N49" r:id="rId225"/>
+    <hyperlink ref="O49" r:id="rId226"/>
+    <hyperlink ref="K50" r:id="rId227"/>
+    <hyperlink ref="L50" r:id="rId228"/>
+    <hyperlink ref="M50" r:id="rId229"/>
+    <hyperlink ref="N50" r:id="rId230"/>
+    <hyperlink ref="O50" r:id="rId231"/>
+    <hyperlink ref="K51" r:id="rId232"/>
+    <hyperlink ref="L51" r:id="rId233"/>
+    <hyperlink ref="M51" r:id="rId234"/>
+    <hyperlink ref="N51" r:id="rId235"/>
+    <hyperlink ref="O51" r:id="rId236"/>
+    <hyperlink ref="K52" r:id="rId237"/>
+    <hyperlink ref="L52" r:id="rId238"/>
+    <hyperlink ref="M52" r:id="rId239"/>
+    <hyperlink ref="N52" r:id="rId240"/>
+    <hyperlink ref="O52" r:id="rId241"/>
+    <hyperlink ref="K53" r:id="rId242"/>
+    <hyperlink ref="L53" r:id="rId243"/>
+    <hyperlink ref="M53" r:id="rId244"/>
+    <hyperlink ref="N53" r:id="rId245"/>
+    <hyperlink ref="O53" r:id="rId246"/>
+    <hyperlink ref="K54" r:id="rId247"/>
+    <hyperlink ref="L54" r:id="rId248"/>
+    <hyperlink ref="M54" r:id="rId249"/>
+    <hyperlink ref="N54" r:id="rId250"/>
+    <hyperlink ref="O54" r:id="rId251"/>
+    <hyperlink ref="K55" r:id="rId252"/>
+    <hyperlink ref="L55" r:id="rId253"/>
+    <hyperlink ref="M55" r:id="rId254"/>
+    <hyperlink ref="N55" r:id="rId255"/>
+    <hyperlink ref="O55" r:id="rId256"/>
+    <hyperlink ref="K56" r:id="rId257"/>
+    <hyperlink ref="L56" r:id="rId258"/>
+    <hyperlink ref="M56" r:id="rId259"/>
+    <hyperlink ref="N56" r:id="rId260"/>
+    <hyperlink ref="O56" r:id="rId261"/>
+    <hyperlink ref="K57" r:id="rId262"/>
+    <hyperlink ref="L57" r:id="rId263"/>
+    <hyperlink ref="M57" r:id="rId264"/>
+    <hyperlink ref="N57" r:id="rId265"/>
+    <hyperlink ref="O57" r:id="rId266"/>
+    <hyperlink ref="K58" r:id="rId267"/>
+    <hyperlink ref="L58" r:id="rId268"/>
+    <hyperlink ref="M58" r:id="rId269"/>
+    <hyperlink ref="N58" r:id="rId270"/>
+    <hyperlink ref="O58" r:id="rId271"/>
+    <hyperlink ref="K59" r:id="rId272"/>
+    <hyperlink ref="L59" r:id="rId273"/>
+    <hyperlink ref="M59" r:id="rId274"/>
+    <hyperlink ref="N59" r:id="rId275"/>
+    <hyperlink ref="O59" r:id="rId276"/>
+    <hyperlink ref="K60" r:id="rId277"/>
+    <hyperlink ref="L60" r:id="rId278"/>
+    <hyperlink ref="M60" r:id="rId279"/>
+    <hyperlink ref="N60" r:id="rId280"/>
+    <hyperlink ref="O60" r:id="rId281"/>
+    <hyperlink ref="K61" r:id="rId282"/>
+    <hyperlink ref="L61" r:id="rId283"/>
+    <hyperlink ref="M61" r:id="rId284"/>
+    <hyperlink ref="N61" r:id="rId285"/>
+    <hyperlink ref="O61" r:id="rId286"/>
+    <hyperlink ref="K62" r:id="rId287"/>
+    <hyperlink ref="L62" r:id="rId288"/>
+    <hyperlink ref="M62" r:id="rId289"/>
+    <hyperlink ref="N62" r:id="rId290"/>
+    <hyperlink ref="O62" r:id="rId291"/>
+    <hyperlink ref="K63" r:id="rId292"/>
+    <hyperlink ref="L63" r:id="rId293"/>
+    <hyperlink ref="M63" r:id="rId294"/>
+    <hyperlink ref="N63" r:id="rId295"/>
+    <hyperlink ref="O63" r:id="rId296"/>
+    <hyperlink ref="K64" r:id="rId297"/>
+    <hyperlink ref="L64" r:id="rId298"/>
+    <hyperlink ref="M64" r:id="rId299"/>
+    <hyperlink ref="N64" r:id="rId300"/>
+    <hyperlink ref="O64" r:id="rId301"/>
+    <hyperlink ref="K65" r:id="rId302"/>
+    <hyperlink ref="L65" r:id="rId303"/>
+    <hyperlink ref="M65" r:id="rId304"/>
+    <hyperlink ref="N65" r:id="rId305"/>
+    <hyperlink ref="O65" r:id="rId306"/>
+    <hyperlink ref="K66" r:id="rId307"/>
+    <hyperlink ref="L66" r:id="rId308"/>
+    <hyperlink ref="M66" r:id="rId309"/>
+    <hyperlink ref="N66" r:id="rId310"/>
+    <hyperlink ref="O66" r:id="rId311"/>
+    <hyperlink ref="K67" r:id="rId312"/>
+    <hyperlink ref="L67" r:id="rId313"/>
+    <hyperlink ref="M67" r:id="rId314"/>
+    <hyperlink ref="N67" r:id="rId315"/>
+    <hyperlink ref="O67" r:id="rId316"/>
+    <hyperlink ref="K68" r:id="rId317"/>
+    <hyperlink ref="L68" r:id="rId318"/>
+    <hyperlink ref="M68" r:id="rId319"/>
+    <hyperlink ref="N68" r:id="rId320"/>
+    <hyperlink ref="O68" r:id="rId321"/>
+    <hyperlink ref="K69" r:id="rId322"/>
+    <hyperlink ref="L69" r:id="rId323"/>
+    <hyperlink ref="M69" r:id="rId324"/>
+    <hyperlink ref="N69" r:id="rId325"/>
+    <hyperlink ref="O69" r:id="rId326"/>
+    <hyperlink ref="K70" r:id="rId327"/>
+    <hyperlink ref="L70" r:id="rId328"/>
+    <hyperlink ref="M70" r:id="rId329"/>
+    <hyperlink ref="N70" r:id="rId330"/>
+    <hyperlink ref="O70" r:id="rId331"/>
+    <hyperlink ref="K71" r:id="rId332"/>
+    <hyperlink ref="L71" r:id="rId333"/>
+    <hyperlink ref="M71" r:id="rId334"/>
+    <hyperlink ref="N71" r:id="rId335"/>
+    <hyperlink ref="O71" r:id="rId336"/>
+    <hyperlink ref="K72" r:id="rId337"/>
+    <hyperlink ref="L72" r:id="rId338"/>
+    <hyperlink ref="M72" r:id="rId339"/>
+    <hyperlink ref="N72" r:id="rId340"/>
+    <hyperlink ref="O72" r:id="rId341"/>
+    <hyperlink ref="K73" r:id="rId342"/>
+    <hyperlink ref="L73" r:id="rId343"/>
+    <hyperlink ref="M73" r:id="rId344"/>
+    <hyperlink ref="N73" r:id="rId345"/>
+    <hyperlink ref="O73" r:id="rId346"/>
+    <hyperlink ref="K74" r:id="rId347"/>
+    <hyperlink ref="L74" r:id="rId348"/>
+    <hyperlink ref="M74" r:id="rId349"/>
+    <hyperlink ref="N74" r:id="rId350"/>
+    <hyperlink ref="O74" r:id="rId351"/>
+    <hyperlink ref="K75" r:id="rId352"/>
+    <hyperlink ref="L75" r:id="rId353"/>
+    <hyperlink ref="M75" r:id="rId354"/>
+    <hyperlink ref="N75" r:id="rId355"/>
+    <hyperlink ref="O75" r:id="rId356"/>
+    <hyperlink ref="K76" r:id="rId357"/>
+    <hyperlink ref="L76" r:id="rId358"/>
+    <hyperlink ref="M76" r:id="rId359"/>
+    <hyperlink ref="N76" r:id="rId360"/>
+    <hyperlink ref="O76" r:id="rId361"/>
+    <hyperlink ref="K77" r:id="rId362"/>
+    <hyperlink ref="L77" r:id="rId363"/>
+    <hyperlink ref="M77" r:id="rId364"/>
+    <hyperlink ref="N77" r:id="rId365"/>
+    <hyperlink ref="O77" r:id="rId366"/>
+    <hyperlink ref="K78" r:id="rId367"/>
+    <hyperlink ref="L78" r:id="rId368"/>
+    <hyperlink ref="M78" r:id="rId369"/>
+    <hyperlink ref="N78" r:id="rId370"/>
+    <hyperlink ref="O78" r:id="rId371"/>
+    <hyperlink ref="K79" r:id="rId372"/>
+    <hyperlink ref="L79" r:id="rId373"/>
+    <hyperlink ref="M79" r:id="rId374"/>
+    <hyperlink ref="N79" r:id="rId375"/>
+    <hyperlink ref="O79" r:id="rId376"/>
+    <hyperlink ref="K80" r:id="rId377"/>
+    <hyperlink ref="L80" r:id="rId378"/>
+    <hyperlink ref="M80" r:id="rId379"/>
+    <hyperlink ref="K81" r:id="rId380"/>
+    <hyperlink ref="L81" r:id="rId381"/>
+    <hyperlink ref="M81" r:id="rId382"/>
+    <hyperlink ref="N81" r:id="rId383"/>
+    <hyperlink ref="O81" r:id="rId384"/>
+    <hyperlink ref="K82" r:id="rId385"/>
+    <hyperlink ref="L82" r:id="rId386"/>
+    <hyperlink ref="M82" r:id="rId387"/>
+    <hyperlink ref="N82" r:id="rId388"/>
+    <hyperlink ref="O82" r:id="rId389"/>
+    <hyperlink ref="K83" r:id="rId390"/>
+    <hyperlink ref="L83" r:id="rId391"/>
+    <hyperlink ref="M83" r:id="rId392"/>
+    <hyperlink ref="N83" r:id="rId393"/>
+    <hyperlink ref="O83" r:id="rId394"/>
+    <hyperlink ref="K84" r:id="rId395"/>
+    <hyperlink ref="L84" r:id="rId396"/>
+    <hyperlink ref="M84" r:id="rId397"/>
+    <hyperlink ref="N84" r:id="rId398"/>
+    <hyperlink ref="O84" r:id="rId399"/>
+    <hyperlink ref="K85" r:id="rId400"/>
+    <hyperlink ref="L85" r:id="rId401"/>
+    <hyperlink ref="M85" r:id="rId402"/>
+    <hyperlink ref="N85" r:id="rId403"/>
+    <hyperlink ref="O85" r:id="rId404"/>
+    <hyperlink ref="K86" r:id="rId405"/>
+    <hyperlink ref="L86" r:id="rId406"/>
+    <hyperlink ref="M86" r:id="rId407"/>
+    <hyperlink ref="N86" r:id="rId408"/>
+    <hyperlink ref="O86" r:id="rId409"/>
+    <hyperlink ref="K87" r:id="rId410"/>
+    <hyperlink ref="L87" r:id="rId411"/>
+    <hyperlink ref="M87" r:id="rId412"/>
+    <hyperlink ref="N87" r:id="rId413"/>
+    <hyperlink ref="O87" r:id="rId414"/>
+    <hyperlink ref="K88" r:id="rId415"/>
+    <hyperlink ref="L88" r:id="rId416"/>
+    <hyperlink ref="M88" r:id="rId417"/>
+    <hyperlink ref="N88" r:id="rId418"/>
+    <hyperlink ref="O88" r:id="rId419"/>
+    <hyperlink ref="K89" r:id="rId420"/>
+    <hyperlink ref="L89" r:id="rId421"/>
+    <hyperlink ref="M89" r:id="rId422"/>
+    <hyperlink ref="N89" r:id="rId423"/>
+    <hyperlink ref="O89" r:id="rId424"/>
+    <hyperlink ref="K90" r:id="rId425"/>
+    <hyperlink ref="L90" r:id="rId426"/>
+    <hyperlink ref="M90" r:id="rId427"/>
+    <hyperlink ref="N90" r:id="rId428"/>
+    <hyperlink ref="O90" r:id="rId429"/>
+    <hyperlink ref="K91" r:id="rId430"/>
+    <hyperlink ref="L91" r:id="rId431"/>
+    <hyperlink ref="M91" r:id="rId432"/>
+    <hyperlink ref="N91" r:id="rId433"/>
+    <hyperlink ref="O91" r:id="rId434"/>
+    <hyperlink ref="K92" r:id="rId435"/>
+    <hyperlink ref="L92" r:id="rId436"/>
+    <hyperlink ref="M92" r:id="rId437"/>
+    <hyperlink ref="N92" r:id="rId438"/>
+    <hyperlink ref="O92" r:id="rId439"/>
+    <hyperlink ref="K93" r:id="rId440"/>
+    <hyperlink ref="L93" r:id="rId441"/>
+    <hyperlink ref="M93" r:id="rId442"/>
+    <hyperlink ref="N93" r:id="rId443"/>
+    <hyperlink ref="O93" r:id="rId444"/>
+    <hyperlink ref="K94" r:id="rId445"/>
+    <hyperlink ref="L94" r:id="rId446"/>
+    <hyperlink ref="M94" r:id="rId447"/>
+    <hyperlink ref="N94" r:id="rId448"/>
+    <hyperlink ref="O94" r:id="rId449"/>
+    <hyperlink ref="K95" r:id="rId450"/>
+    <hyperlink ref="L95" r:id="rId451"/>
+    <hyperlink ref="M95" r:id="rId452"/>
+    <hyperlink ref="N95" r:id="rId453"/>
+    <hyperlink ref="O95" r:id="rId454"/>
+    <hyperlink ref="K96" r:id="rId455"/>
+    <hyperlink ref="L96" r:id="rId456"/>
+    <hyperlink ref="M96" r:id="rId457"/>
+    <hyperlink ref="N96" r:id="rId458"/>
+    <hyperlink ref="O96" r:id="rId459"/>
+    <hyperlink ref="K97" r:id="rId460"/>
+    <hyperlink ref="L97" r:id="rId461"/>
+    <hyperlink ref="M97" r:id="rId462"/>
+    <hyperlink ref="N97" r:id="rId463"/>
+    <hyperlink ref="O97" r:id="rId464"/>
+    <hyperlink ref="K98" r:id="rId465"/>
+    <hyperlink ref="L98" r:id="rId466"/>
+    <hyperlink ref="M98" r:id="rId467"/>
+    <hyperlink ref="N98" r:id="rId468"/>
+    <hyperlink ref="O98" r:id="rId469"/>
+    <hyperlink ref="K99" r:id="rId470"/>
+    <hyperlink ref="L99" r:id="rId471"/>
+    <hyperlink ref="M99" r:id="rId472"/>
+    <hyperlink ref="N99" r:id="rId473"/>
+    <hyperlink ref="O99" r:id="rId474"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>